<commit_message>
Fix master story sheets
</commit_message>
<xml_diff>
--- a/sheets/master_story.xlsx
+++ b/sheets/master_story.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="15600"/>
   </bookViews>
   <sheets>
-    <sheet name="01_02" sheetId="1" r:id="rId4"/>
+    <sheet name="01_02" sheetId="2" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
-  <si>
-    <t>表 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>type</t>
   </si>
@@ -86,68 +85,35 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="ヒラギノ角ゴ ProN W3"/>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="ヒラギノ角ゴ ProN W6"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="ヒラギノ角ゴ ProN W3"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -155,154 +121,103 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ff3c4a60"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FF3C4A60"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -494,7 +409,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -503,7 +418,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -512,7 +427,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -521,7 +436,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -530,7 +445,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -539,7 +454,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -651,8 +566,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -660,14 +575,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -686,7 +601,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -694,7 +609,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -722,7 +637,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -748,7 +663,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -774,7 +689,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -800,7 +715,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -826,7 +741,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -852,7 +767,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -878,7 +793,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -904,7 +819,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -930,7 +845,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -943,9 +858,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -961,7 +882,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -980,7 +901,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1006,7 +927,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1032,7 +953,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1058,7 +979,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1084,7 +1005,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1110,7 +1031,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1136,7 +1057,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1162,7 +1083,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1188,7 +1109,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1214,7 +1135,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,9 +1148,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1242,7 +1169,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1261,7 +1188,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1291,7 +1218,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1317,7 +1244,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1343,7 +1270,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1369,7 +1296,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1395,7 +1322,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1421,7 +1348,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1447,7 +1374,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1473,7 +1400,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1499,7 +1426,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1512,276 +1439,194 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="83.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="1" customWidth="1"/>
-    <col min="7" max="256" width="12.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="1"/>
+    <col min="2" max="2" width="69.59765625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" ht="18.5" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" t="s" s="7">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s" s="7">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s" s="7">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="7">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="23.55" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s" s="9">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" ht="23.35" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s" s="9">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" ht="23.35" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s" s="9">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="6" ht="23.35" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s" s="11">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" ht="23.35" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s" s="11">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" ht="23.35" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s" s="11">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" ht="23.35" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s" s="11">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" ht="23.35" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s" s="11">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" ht="23.85" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="8">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s" s="11">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" ht="23.85" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="8">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s" s="11">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" ht="23.35" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s" s="11">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" ht="23.35" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="8">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s" s="11">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" ht="23.35" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="8">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s" s="11">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" ht="23.35" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s" s="11">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" ht="23.35" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="8">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s" s="11">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" ht="23.35" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="8">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s" s="11">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" ht="23.85" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="8">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s" s="11">
-        <v>22</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
-  </headerFooter>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create story sheets for scrap field (empty)
</commit_message>
<xml_diff>
--- a/sheets/master_story.xlsx
+++ b/sheets/master_story.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="15600"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="15600" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="01_02" sheetId="2" r:id="rId1"/>
+    <sheet name="01_01" sheetId="3" r:id="rId1"/>
+    <sheet name="01_02" sheetId="2" r:id="rId2"/>
+    <sheet name="01_03" sheetId="4" r:id="rId3"/>
+    <sheet name="01_04" sheetId="5" r:id="rId4"/>
+    <sheet name="01_05" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>type</t>
   </si>
@@ -1458,10 +1462,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1629,4 +1670,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>